<commit_message>
Match electors and convert to destination format
</commit_message>
<xml_diff>
--- a/tests/test_combined_data.xlsx
+++ b/tests/test_combined_data.xlsx
@@ -31,6 +31,27 @@
     <t xml:space="preserve">Elector Markers</t>
   </si>
   <si>
+    <t xml:space="preserve">Forename</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PostCode</t>
+  </si>
+  <si>
     <t xml:space="preserve">Month first seen on roll</t>
   </si>
   <si>
@@ -46,27 +67,6 @@
     <t xml:space="preserve">GP member</t>
   </si>
   <si>
-    <t xml:space="preserve">Forename</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PostCode</t>
-  </si>
-  <si>
     <t xml:space="preserve">Do not knock</t>
   </si>
   <si>
@@ -109,21 +109,21 @@
     <t xml:space="preserve">E1 1AA</t>
   </si>
   <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flat 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Foo Road</t>
+  </si>
+  <si>
     <t xml:space="preserve">x</t>
   </si>
   <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flat 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Foo Road</t>
-  </si>
-  <si>
     <t xml:space="preserve">DNK</t>
   </si>
   <si>
@@ -142,24 +142,24 @@
     <t xml:space="preserve">L</t>
   </si>
   <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the bin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flat 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Foo Road</t>
+  </si>
+  <si>
     <t xml:space="preserve">v</t>
   </si>
   <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In the bin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flat 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 Foo Road</t>
-  </si>
-  <si>
     <t xml:space="preserve">Labour</t>
   </si>
   <si>
@@ -175,31 +175,31 @@
     <t xml:space="preserve">AB</t>
   </si>
   <si>
+    <t xml:space="preserve">J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I</t>
+  </si>
+  <si>
     <t xml:space="preserve">2021 May</t>
   </si>
   <si>
-    <t xml:space="preserve">J</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I</t>
-  </si>
-  <si>
     <t xml:space="preserve">A/B/C/D/E</t>
   </si>
   <si>
     <t xml:space="preserve">Some notes</t>
   </si>
   <si>
+    <t xml:space="preserve">P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Bar Road</t>
+  </si>
+  <si>
     <t xml:space="preserve">2022 December</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Bar Road</t>
   </si>
 </sst>
 </file>
@@ -317,10 +317,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X7"/>
+  <dimension ref="A1:AC7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X14" activeCellId="0" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -328,11 +328,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="5.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="9.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="6.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="8.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="6"/>
@@ -410,6 +410,11 @@
         <v>22</v>
       </c>
       <c r="X1" s="1"/>
+      <c r="Y1" s="0"/>
+      <c r="Z1" s="0"/>
+      <c r="AA1" s="0"/>
+      <c r="AB1" s="0"/>
+      <c r="AC1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -418,23 +423,23 @@
       <c r="B2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="D2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -444,32 +449,32 @@
       <c r="B3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="D3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="M3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" s="0" t="s">
+      <c r="N3" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>28</v>
       </c>
       <c r="P3" s="0" t="s">
         <v>34</v>
@@ -506,35 +511,35 @@
       <c r="C4" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="D4" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>44</v>
-      </c>
       <c r="M4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="N4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" s="0" t="s">
-        <v>28</v>
       </c>
       <c r="P4" s="0" t="s">
         <v>34</v>
@@ -565,29 +570,29 @@
       <c r="B5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="D5" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="0" t="s">
+      <c r="M5" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="O5" s="0" t="s">
         <v>36</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O5" s="0" t="s">
-        <v>28</v>
       </c>
       <c r="S5" s="0" t="s">
         <v>38</v>
@@ -612,23 +617,23 @@
       <c r="D6" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6" s="0" t="n">
         <v>2</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O6" s="0" t="s">
-        <v>28</v>
       </c>
       <c r="T6" s="0" t="s">
         <v>54</v>
@@ -650,23 +655,23 @@
       <c r="C7" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="F7" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>27</v>
+      </c>
       <c r="J7" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="K7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Compare names without non-letter characters
This should help us match people who've had their non-letter characters
change. For example, I've seen ' become ` in a name in a way where it
was obvious that it was the same person.
</commit_message>
<xml_diff>
--- a/tests/test_combined_data.xlsx
+++ b/tests/test_combined_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
   <si>
     <t xml:space="preserve">Elector Number Prefix</t>
   </si>
@@ -100,64 +100,67 @@
     <t xml:space="preserve">BW1</t>
   </si>
   <si>
+    <t xml:space="preserve">O’A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Foo Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">London</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E1 1AA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 December</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flat 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Foo Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the bin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNK</t>
+  </si>
+  <si>
     <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 Foo Road</t>
-  </si>
-  <si>
-    <t xml:space="preserve">London</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E1 1AA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022 December</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flat 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 Foo Road</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In the bin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DNK</t>
   </si>
   <si>
     <t xml:space="preserve">Labour</t>
@@ -211,7 +214,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -241,6 +244,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -284,7 +292,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -294,6 +302,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -324,8 +336,8 @@
   </sheetPr>
   <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -421,7 +433,7 @@
       <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="0"/>
+      <c r="Z1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -433,7 +445,7 @@
       <c r="C2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -519,7 +531,7 @@
       <c r="X3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="Y3" s="3" t="n">
+      <c r="Y3" s="4" t="n">
         <v>44562</v>
       </c>
     </row>
@@ -573,18 +585,18 @@
         <v>45</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="W4" s="1" t="n">
         <v>5</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y4" s="3" t="n">
+        <v>46</v>
+      </c>
+      <c r="Y4" s="4" t="n">
         <v>44561</v>
       </c>
     </row>
@@ -602,7 +614,7 @@
         <v>40</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>28</v>
@@ -615,7 +627,7 @@
         <v>30</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N5" s="1" t="n">
         <v>2</v>
@@ -630,15 +642,15 @@
         <v>40</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y5" s="4" t="n">
+        <v>52</v>
+      </c>
+      <c r="Y5" s="5" t="n">
         <v>44595</v>
       </c>
     </row>
@@ -652,14 +664,14 @@
       <c r="C6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="4" t="n">
         <v>36526</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>28</v>
@@ -678,13 +690,13 @@
         <v>0</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>40</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -701,10 +713,10 @@
         <v>40</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>28</v>
@@ -717,7 +729,7 @@
         <v>30</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -734,13 +746,13 @@
         <v>43</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>39</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>